<commit_message>
Projection images and data updates
</commit_message>
<xml_diff>
--- a/applications/us_states/US-cities-data-group1/Los-Angeles_projections.xlsx
+++ b/applications/us_states/US-cities-data-group1/Los-Angeles_projections.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom.walsh\Documents\GitHub\covasim-australia\applications\us_states\US-cities-data-group1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B40D93-3C39-47C2-8121-4315FF56851E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A917859E-D2F7-4232-9C50-E971F34675C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-7380" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projections" sheetId="1" r:id="rId1"/>
+    <sheet name="1520" sheetId="2" r:id="rId2"/>
+    <sheet name="1020" sheetId="4" r:id="rId3"/>
+    <sheet name="1525" sheetId="3" r:id="rId4"/>
+    <sheet name="2030" sheetId="5" r:id="rId5"/>
+    <sheet name="2040" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="9">
   <si>
     <t>Mid Sep – end Oct</t>
   </si>
@@ -128,6 +133,166 @@
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2E581DC7-48C1-4B72-BAE3-FC9E1F3FB6C3}" name="Table13" displayName="Table13" ref="A1:X4" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{98DAD4A7-D7C8-425A-B29C-6436DA53FAB0}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{41DC2CF8-3B51-41AE-A0E6-2303BAE7A01D}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{80A689C3-120E-4B60-A58C-A9D3F06EC5A1}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{FEC2A6DB-81A0-4E03-AB2D-C78036302C41}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{285D1888-712E-4509-9A79-5D339C0C0451}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{CD3E2D9F-173B-4457-AA2F-D44B84E9FD15}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{CE84809C-6DF4-451B-B7B3-7324ACB7CC46}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{737443FF-FA53-4A09-9B46-CC536F3D92AA}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{85F5BD78-EF1E-44E8-88EB-45A05B85D919}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{14B74127-8AEB-47F3-988B-C3209E4C3096}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{DBC4CAC4-6F21-45CE-B3FC-CF36D2992E09}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{F74E623D-1528-4D65-84AD-4E0D578DFFD3}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{B4666F10-239A-458E-A780-F89A0FE091E9}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{1DB3DDEA-5F06-443E-93A0-6BD2498267EB}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{B5B9ADFD-CB06-405B-A47C-6D1C593DEABF}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{E825AC4D-B894-46C3-8AC2-6CDA99FA7465}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{15111B1F-34C7-497F-B1AF-826548AB5B48}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{9CA47ECA-E928-4465-A066-483DE325716F}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{727F9C09-33A7-4DAD-BCA5-13421D90EC66}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{74A63260-C179-4532-A1FE-50326115878B}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{21E5F82A-1A60-40BB-9D98-D5D62D5A9DE0}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{63F31D26-C720-4B17-9851-FCC57DBD81A8}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{27D17520-21A8-4B28-95CF-E49292FE9694}" name="Column23"/>
+    <tableColumn id="24" xr3:uid="{6D48C7A3-26E0-48CD-BA46-EF5859317AD4}" name="Column24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F23BA31B-978B-4EA7-AA22-DC8CA5C4ADF0}" name="Table15" displayName="Table15" ref="A1:X4" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{02B63643-0286-4494-BC75-9D93F1E5169B}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{BBA6F992-5B3A-44B1-A4C1-3562633F0FD6}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{61B84845-71C5-4C83-B978-B47C89E8BA71}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{B4D12B00-FA3D-439C-998B-F3A80D0A8704}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{192B0F44-58CC-43E9-88F0-3534499E2EA1}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00E74B27-727F-41AC-81B5-E9E692056D03}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{41E1675A-483F-408B-AFCA-600EC99AF1AA}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{845744EF-A8C1-4A4F-98A8-B973CBECF13E}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{829053B3-4368-49C8-A72A-FE222E568A13}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{F2061641-F657-44F4-82DD-35304F0D8983}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{100AC9A7-E3A5-4BBC-8203-4638EEA966D4}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{EF18EA3F-9246-4751-997A-C7572BDFAE81}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{B9455F5A-BE30-463E-9A3A-B99BE477541F}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{D5BE3504-B8A0-477B-8037-0A2DDFFDACAA}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{53918248-8EB9-4373-A572-63A9395B6A6D}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{49173939-4571-4773-93A0-5D31761995A0}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{C6406238-CB4D-4324-B5BA-18B45908455F}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{5A821751-FE5E-4721-B638-D03CCAF45FF1}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{3BD25C54-B648-4240-8B57-E5DB71D1F258}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{9D034C4C-A145-4F6F-87D7-1408654D3365}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{0974652E-A7A9-47EB-9117-DCA72DCF983C}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{AABC343B-6D3D-493F-810C-2A0806AE15E9}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{E6790B55-33D9-4BAD-96CF-652E92D08E75}" name="Column23"/>
+    <tableColumn id="24" xr3:uid="{41B549A8-DCA4-486C-BBB0-3A4E762E0F46}" name="Column24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B3188738-4279-4AB3-9E26-1D3BF9C22408}" name="Table14" displayName="Table14" ref="A1:X4" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{8049EE72-A8D0-4194-8505-392B229DB614}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{328D9EDE-98AC-4A40-A3F9-3B24837FA1C2}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{AB664C96-33CC-4F0A-B3BB-A0C007E9EA9D}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{1AA9E19B-92AA-4CC5-8919-D84239205FF2}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{03A4D908-B08A-4044-9575-A1C02B5404FA}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{7FEAF5E1-F6D7-42CA-B1F6-86772732ACC7}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{52596897-0DA2-4630-8A4D-458BBB466B9B}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{31A85B9F-F5F3-4BAB-815A-A0CC6A1B2F99}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{5DA40315-BB4F-494E-BC77-F2F493B5D48A}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{DA4AABD8-BC2C-4CB0-A9C4-D6DDFAB693B7}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{76B73958-245A-4520-964C-275D9BD004BB}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{3D333933-21DE-4018-8A20-D11576FD2375}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{B901917F-BA57-496C-8E7A-8D3FDD4136B9}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{608A3271-8B14-4106-98BC-E27FF02BFD98}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{115243A6-C09C-4F4D-8395-DC5473CC85A8}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{B40B1FDF-DDD5-4DDE-84BE-28B23E7A9387}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{147DD8B4-2A2E-45FD-9FA2-7C132277250D}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{9F3D581D-D152-44BB-8D23-5B54D6F73AFA}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{EB6E9049-C551-4521-975C-7BB66883C35F}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{F5372511-2DBB-41EF-A769-D21F0E96AB29}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{3D6C1404-7CE6-4350-A429-93916F0FAFD2}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{E80C7138-0CCF-4B18-9EF0-2721CA42CB1A}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{BFE1CD67-7B6C-4B51-9052-01FD2020193A}" name="Column23"/>
+    <tableColumn id="24" xr3:uid="{8649B412-3A28-408A-A9D7-BE935F440F28}" name="Column24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E6F6D556-812B-4B1A-8A9B-92132EACE5B6}" name="Table16" displayName="Table16" ref="A1:X4" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{F4E52C3A-8B34-4685-AF74-F7B28BA0249D}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{8C57D1BB-FE0E-423B-B8FE-569A96BD2137}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{FA2C865E-4235-43A7-93CD-A06FB27537A1}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{885E6307-79CC-45AD-B456-DBFC20E14B4A}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{4FC2A327-CB47-4DF5-B8A6-6CACC365F1F7}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{A5C7D548-84EE-4BEF-B1B3-FF87286208C2}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{B9C42121-3A0A-4552-96A5-46F327B646C0}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{F2C6B200-6884-4821-947C-373EB345EFC8}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{B79C693E-6A0D-4EEC-BFB3-8238B5A3548A}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{A0C1AD01-7756-46D3-99F1-D40EAFBFA2F1}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{D75120D3-636D-411E-AF53-056A1FBA888F}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{01983899-F7C0-4929-B7E8-E46B95782372}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{247CBF30-6B2F-41B2-B8A7-2E7849A2447E}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{5358D32C-073C-4445-9AD4-0A019413F3F7}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{03CC55A6-9AEF-41E5-8A5D-FA7D8A8E4842}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{7B6E73E7-228A-4B4B-AC1B-376CD0159A87}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{3209E367-AA0C-4831-98BB-4C5A66840478}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{74CC11F9-396A-4FC9-A923-3281770F444F}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{75E6DD07-C1F6-498C-A9D6-DBB5C39A885D}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{389DBC37-8C3D-4529-976F-894A30D2D678}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{883DAA5B-45F2-49A6-ABE6-08766CB5F366}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{30A75650-F694-4FAC-9FA0-3E92C3DE99CF}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{10997C3E-A2E8-4B6F-A4C9-7BB97F2DC6E5}" name="Column23"/>
+    <tableColumn id="24" xr3:uid="{144B6086-B79B-4390-A566-DDAC2791292F}" name="Column24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{922B2D3B-C4BB-4B40-88EE-B89CA5F1B8B1}" name="Table17" displayName="Table17" ref="A1:X4" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{C46982F0-C7FF-4269-AE9A-CF943C0D8609}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{5B56B038-DBB0-467F-94C6-DD9CB1740BC3}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{799FA8A7-C34C-413E-969F-7936D15DBC41}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{7782A6E0-956B-43FF-A36F-F4C1A5367862}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{63AD5F3F-6C4B-4492-B40F-4FBDB64B14F7}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{871F48FA-5792-41E5-B49E-A91A831C8949}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{EDFD347F-7570-4AC0-BD72-FA19AFAC2BE6}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{1397A254-964C-449A-B7CE-084B30652077}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{A728CA0B-1A3E-463A-A70B-C1DAA37D981C}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{45FE04DF-97C9-407B-807C-F051F962CAE5}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{74B445A7-CAF7-4DC0-A2AB-5BBAFFE96B99}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{3ED85D94-2765-4075-8B75-693D484B6338}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{626820BB-B60F-4DA4-8A03-FA92D1BC1578}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{4FBF93BC-5CAC-42F2-B29F-2D012BED3BEB}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{FC171527-A4D8-4893-9E4F-1DAE3F88CDE4}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{802B8655-C048-47C6-8E43-172709AEFD2A}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{56DDAFB1-29ED-44AD-99B5-27D6F04BA989}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{FEBDFF6A-E967-4046-A30B-966EEDD86F8C}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{7048EC06-106F-4BD3-80FB-3FE974078312}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{6AE3A0C6-A2AE-4837-AF1C-8876C3E0C46F}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{F959C654-87AC-4F2C-82B7-2AEE7D00114D}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{D2BAF137-0313-4403-99AE-63BFE219CE64}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{8F749207-6C80-4B0E-B97F-06F2350AD561}" name="Column23"/>
+    <tableColumn id="24" xr3:uid="{2C52A8C7-C664-4127-83A6-66A0E3C3AE2A}" name="Column24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -456,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
@@ -651,4 +816,1004 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB905020-CFFC-43C4-8F35-1956D596A124}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>127405</v>
+      </c>
+      <c r="B4">
+        <v>9821</v>
+      </c>
+      <c r="C4">
+        <v>203534</v>
+      </c>
+      <c r="D4">
+        <v>2.0824640066187832</v>
+      </c>
+      <c r="E4">
+        <v>0.16052716300268599</v>
+      </c>
+      <c r="F4">
+        <v>3.326815695200541</v>
+      </c>
+      <c r="G4">
+        <v>0.40873002973990669</v>
+      </c>
+      <c r="H4">
+        <v>6.3495665114905286E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.54476285384518985</v>
+      </c>
+      <c r="J4">
+        <v>0.1244615894085494</v>
+      </c>
+      <c r="K4">
+        <v>7.8408138148740772E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.15311765813341219</v>
+      </c>
+      <c r="M4">
+        <v>182715</v>
+      </c>
+      <c r="N4">
+        <v>2277</v>
+      </c>
+      <c r="O4">
+        <v>267824</v>
+      </c>
+      <c r="P4">
+        <v>3.1222824772977078</v>
+      </c>
+      <c r="Q4">
+        <v>3.8912470757413921E-2</v>
+      </c>
+      <c r="R4">
+        <v>4.5766377952083994</v>
+      </c>
+      <c r="S4">
+        <v>0.48364048847583307</v>
+      </c>
+      <c r="T4">
+        <v>1.6305325703302849E-2</v>
+      </c>
+      <c r="U4">
+        <v>0.63512198367143569</v>
+      </c>
+      <c r="V4">
+        <v>0.1794408419962282</v>
+      </c>
+      <c r="W4">
+        <v>7.9122498798189028E-2</v>
+      </c>
+      <c r="X4">
+        <v>0.26093613875541388</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6798C0D-259A-4D96-BAA3-3D3349A1344A}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1090</v>
+      </c>
+      <c r="B4">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <v>185374</v>
+      </c>
+      <c r="D4">
+        <v>1.7820542053166782E-2</v>
+      </c>
+      <c r="E4">
+        <v>7.7298131378799955E-4</v>
+      </c>
+      <c r="F4">
+        <v>3.0299814287217139</v>
+      </c>
+      <c r="G4">
+        <v>8.4118554735752877E-3</v>
+      </c>
+      <c r="H4">
+        <v>3.8474183039221692E-4</v>
+      </c>
+      <c r="I4">
+        <v>0.50905222358540625</v>
+      </c>
+      <c r="J4">
+        <v>5.7651909742594862E-2</v>
+      </c>
+      <c r="K4">
+        <v>5.6099837881105979E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.1185157130376088</v>
+      </c>
+      <c r="M4">
+        <v>66</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>631697</v>
+      </c>
+      <c r="P4">
+        <v>1.1335575416101271E-3</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>10.794553667357571</v>
+      </c>
+      <c r="S4">
+        <v>2.742477923250307E-4</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0.87415150878212944</v>
+      </c>
+      <c r="V4">
+        <v>5.771143979671553E-2</v>
+      </c>
+      <c r="W4">
+        <v>5.6099837881105979E-2</v>
+      </c>
+      <c r="X4">
+        <v>0.31052640754486532</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AA033E-F3A0-44AC-9F57-97C9D322B371}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>171403</v>
+      </c>
+      <c r="B4">
+        <v>9760</v>
+      </c>
+      <c r="C4">
+        <v>675191</v>
+      </c>
+      <c r="D4">
+        <v>2.8016220705041812</v>
+      </c>
+      <c r="E4">
+        <v>0.1595349487986345</v>
+      </c>
+      <c r="F4">
+        <v>11.036149243533581</v>
+      </c>
+      <c r="G4">
+        <v>0.49524987639521612</v>
+      </c>
+      <c r="H4">
+        <v>6.9324042155150936E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.87409685284055882</v>
+      </c>
+      <c r="J4">
+        <v>0.13941015684843541</v>
+      </c>
+      <c r="K4">
+        <v>7.7777946565367795E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.32446218456915321</v>
+      </c>
+      <c r="M4">
+        <v>254983</v>
+      </c>
+      <c r="N4">
+        <v>4044</v>
+      </c>
+      <c r="O4">
+        <v>474935</v>
+      </c>
+      <c r="P4">
+        <v>4.3571975059596237</v>
+      </c>
+      <c r="Q4">
+        <v>6.9120974781133007E-2</v>
+      </c>
+      <c r="R4">
+        <v>8.1157779883753598</v>
+      </c>
+      <c r="S4">
+        <v>0.58443905029500631</v>
+      </c>
+      <c r="T4">
+        <v>2.5229392745206119E-2</v>
+      </c>
+      <c r="U4">
+        <v>0.84272727272727277</v>
+      </c>
+      <c r="V4">
+        <v>0.21596404539816069</v>
+      </c>
+      <c r="W4">
+        <v>7.9300113960030019E-2</v>
+      </c>
+      <c r="X4">
+        <v>0.45005218456915341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C3733A-5F44-4A92-BDB8-2777F7508648}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>360851</v>
+      </c>
+      <c r="B4">
+        <v>9445</v>
+      </c>
+      <c r="C4">
+        <v>160437</v>
+      </c>
+      <c r="D4">
+        <v>5.8981866497943694</v>
+      </c>
+      <c r="E4">
+        <v>0.15438752282634721</v>
+      </c>
+      <c r="F4">
+        <v>2.6223852732473119</v>
+      </c>
+      <c r="G4">
+        <v>2672912</v>
+      </c>
+      <c r="H4">
+        <v>271004</v>
+      </c>
+      <c r="I4">
+        <v>1761673</v>
+      </c>
+      <c r="J4">
+        <v>0.20759671752758591</v>
+      </c>
+      <c r="K4">
+        <v>8.1940611722348414E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.1279713615017129</v>
+      </c>
+      <c r="M4">
+        <v>396559</v>
+      </c>
+      <c r="N4">
+        <v>1987</v>
+      </c>
+      <c r="O4">
+        <v>467756</v>
+      </c>
+      <c r="P4">
+        <v>6.7764746361989134</v>
+      </c>
+      <c r="Q4">
+        <v>3.3962846601531788E-2</v>
+      </c>
+      <c r="R4">
+        <v>7.9931098937807139</v>
+      </c>
+      <c r="S4">
+        <v>3042486</v>
+      </c>
+      <c r="T4">
+        <v>57150</v>
+      </c>
+      <c r="U4">
+        <v>3039111</v>
+      </c>
+      <c r="V4">
+        <v>0.33387734067149238</v>
+      </c>
+      <c r="W4">
+        <v>8.2610180028371907E-2</v>
+      </c>
+      <c r="X4">
+        <v>0.26903181610806098</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C2850E-7033-46DA-B7BF-AFCBB02F3D0D}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>225186</v>
+      </c>
+      <c r="B4">
+        <v>8635</v>
+      </c>
+      <c r="C4">
+        <v>629548</v>
+      </c>
+      <c r="D4">
+        <v>3.680714265568704</v>
+      </c>
+      <c r="E4">
+        <v>0.14114708742828941</v>
+      </c>
+      <c r="F4">
+        <v>10.290101399571981</v>
+      </c>
+      <c r="G4">
+        <v>0.57426257685746884</v>
+      </c>
+      <c r="H4">
+        <v>5.8683342281583492E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.87622591438421837</v>
+      </c>
+      <c r="J4">
+        <v>0.15668990569731939</v>
+      </c>
+      <c r="K4">
+        <v>7.5149543088103579E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.29318494764459002</v>
+      </c>
+      <c r="M4">
+        <v>352156</v>
+      </c>
+      <c r="N4">
+        <v>3668</v>
+      </c>
+      <c r="O4">
+        <v>628848</v>
+      </c>
+      <c r="P4">
+        <v>6.0177130078879983</v>
+      </c>
+      <c r="Q4">
+        <v>6.2691728936098839E-2</v>
+      </c>
+      <c r="R4">
+        <v>10.74587195943556</v>
+      </c>
+      <c r="S4">
+        <v>0.7076951029947175</v>
+      </c>
+      <c r="T4">
+        <v>2.4082554297173001E-2</v>
+      </c>
+      <c r="U4">
+        <v>0.92920521528906463</v>
+      </c>
+      <c r="V4">
+        <v>0.28532059334539078</v>
+      </c>
+      <c r="W4">
+        <v>7.6314530158041627E-2</v>
+      </c>
+      <c r="X4">
+        <v>0.46195494764459011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>